<commit_message>
added some figures to quality
</commit_message>
<xml_diff>
--- a/data/flea_dog_cat_length_weight.xlsx
+++ b/data/flea_dog_cat_length_weight.xlsx
@@ -401,7 +401,7 @@
         <v>16.93</v>
       </c>
       <c r="E2" t="n">
-        <v>68.5607030828682</v>
+        <v>68.56</v>
       </c>
     </row>
     <row r="3">
@@ -418,7 +418,7 @@
         <v>16.22</v>
       </c>
       <c r="E3" t="n">
-        <v>131.663962463075</v>
+        <v>131.66</v>
       </c>
     </row>
     <row r="4">
@@ -435,7 +435,7 @@
         <v>18.96</v>
       </c>
       <c r="E4" t="n">
-        <v>94.6300466572861</v>
+        <v>94.63</v>
       </c>
     </row>
     <row r="5">
@@ -452,7 +452,7 @@
         <v>19.83</v>
       </c>
       <c r="E5" t="n">
-        <v>110.037620806241</v>
+        <v>110.04</v>
       </c>
     </row>
     <row r="6">
@@ -469,7 +469,7 @@
         <v>17.37</v>
       </c>
       <c r="E6" t="n">
-        <v>103.202381557306</v>
+        <v>103.2</v>
       </c>
     </row>
     <row r="7">
@@ -486,7 +486,7 @@
         <v>14.45</v>
       </c>
       <c r="E7" t="n">
-        <v>326.905571938527</v>
+        <v>326.91</v>
       </c>
     </row>
     <row r="8">
@@ -503,7 +503,7 @@
         <v>15.46</v>
       </c>
       <c r="E8" t="n">
-        <v>360.895299014955</v>
+        <v>360.9</v>
       </c>
     </row>
     <row r="9">
@@ -520,7 +520,7 @@
         <v>15.81</v>
       </c>
       <c r="E9" t="n">
-        <v>21.1496681345285</v>
+        <v>21.15</v>
       </c>
     </row>
     <row r="10">
@@ -537,7 +537,7 @@
         <v>19.14</v>
       </c>
       <c r="E10" t="n">
-        <v>203.734455254478</v>
+        <v>203.73</v>
       </c>
     </row>
     <row r="11">
@@ -554,7 +554,7 @@
         <v>15.72</v>
       </c>
       <c r="E11" t="n">
-        <v>878.640460495332</v>
+        <v>878.64</v>
       </c>
     </row>
     <row r="12">
@@ -571,7 +571,7 @@
         <v>14.65</v>
       </c>
       <c r="E12" t="n">
-        <v>338.424763258297</v>
+        <v>338.42</v>
       </c>
     </row>
     <row r="13">
@@ -588,7 +588,7 @@
         <v>17.21</v>
       </c>
       <c r="E13" t="n">
-        <v>81.7145993247279</v>
+        <v>81.71</v>
       </c>
     </row>
     <row r="14">
@@ -605,7 +605,7 @@
         <v>14.07</v>
       </c>
       <c r="E14" t="n">
-        <v>520.188781457742</v>
+        <v>520.19</v>
       </c>
     </row>
     <row r="15">
@@ -622,7 +622,7 @@
         <v>15.5</v>
       </c>
       <c r="E15" t="n">
-        <v>208.102243200523</v>
+        <v>208.1</v>
       </c>
     </row>
     <row r="16">
@@ -639,7 +639,7 @@
         <v>15.37</v>
       </c>
       <c r="E16" t="n">
-        <v>377.381338405879</v>
+        <v>377.38</v>
       </c>
     </row>
     <row r="17">
@@ -656,7 +656,7 @@
         <v>14.79</v>
       </c>
       <c r="E17" t="n">
-        <v>95.5500213810692</v>
+        <v>95.55</v>
       </c>
     </row>
     <row r="18">
@@ -673,7 +673,7 @@
         <v>15.51</v>
       </c>
       <c r="E18" t="n">
-        <v>191.668625005596</v>
+        <v>191.67</v>
       </c>
     </row>
     <row r="19">
@@ -690,7 +690,7 @@
         <v>16.33</v>
       </c>
       <c r="E19" t="n">
-        <v>92.6068959340921</v>
+        <v>92.61</v>
       </c>
     </row>
     <row r="20">
@@ -707,7 +707,7 @@
         <v>16.04</v>
       </c>
       <c r="E20" t="n">
-        <v>340.666860079945</v>
+        <v>340.67</v>
       </c>
     </row>
     <row r="21">
@@ -724,7 +724,7 @@
         <v>16.57</v>
       </c>
       <c r="E21" t="n">
-        <v>70.3109450046642</v>
+        <v>70.31</v>
       </c>
     </row>
     <row r="22">
@@ -741,7 +741,7 @@
         <v>14.33</v>
       </c>
       <c r="E22" t="n">
-        <v>115.371763451043</v>
+        <v>115.37</v>
       </c>
     </row>
     <row r="23">
@@ -758,7 +758,7 @@
         <v>16.29</v>
       </c>
       <c r="E23" t="n">
-        <v>38.6548692308782</v>
+        <v>38.65</v>
       </c>
     </row>
     <row r="24">
@@ -775,7 +775,7 @@
         <v>17.31</v>
       </c>
       <c r="E24" t="n">
-        <v>383.502289367727</v>
+        <v>383.5</v>
       </c>
     </row>
     <row r="25">
@@ -792,7 +792,7 @@
         <v>15.45</v>
       </c>
       <c r="E25" t="n">
-        <v>160.120318685478</v>
+        <v>160.12</v>
       </c>
     </row>
     <row r="26">
@@ -809,7 +809,7 @@
         <v>19.64</v>
       </c>
       <c r="E26" t="n">
-        <v>232.358316218593</v>
+        <v>232.36</v>
       </c>
     </row>
     <row r="27">
@@ -826,7 +826,7 @@
         <v>17.51</v>
       </c>
       <c r="E27" t="n">
-        <v>72.8777808918264</v>
+        <v>72.88</v>
       </c>
     </row>
     <row r="28">
@@ -843,7 +843,7 @@
         <v>14.84</v>
       </c>
       <c r="E28" t="n">
-        <v>158.019270176603</v>
+        <v>158.02</v>
       </c>
     </row>
     <row r="29">
@@ -860,7 +860,7 @@
         <v>14.18</v>
       </c>
       <c r="E29" t="n">
-        <v>459.033173485359</v>
+        <v>459.03</v>
       </c>
     </row>
     <row r="30">
@@ -877,7 +877,7 @@
         <v>13.46</v>
       </c>
       <c r="E30" t="n">
-        <v>72.5606942162136</v>
+        <v>72.56</v>
       </c>
     </row>
     <row r="31">
@@ -894,7 +894,7 @@
         <v>17.43</v>
       </c>
       <c r="E31" t="n">
-        <v>1523.09723340079</v>
+        <v>1523.1</v>
       </c>
     </row>
     <row r="32">
@@ -911,7 +911,7 @@
         <v>15.06</v>
       </c>
       <c r="E32" t="n">
-        <v>39.487775162613</v>
+        <v>39.49</v>
       </c>
     </row>
     <row r="33">
@@ -928,7 +928,7 @@
         <v>17.84</v>
       </c>
       <c r="E33" t="n">
-        <v>188.294108385254</v>
+        <v>188.29</v>
       </c>
     </row>
     <row r="34">
@@ -945,7 +945,7 @@
         <v>16.14</v>
       </c>
       <c r="E34" t="n">
-        <v>102.661620152113</v>
+        <v>102.66</v>
       </c>
     </row>
     <row r="35">
@@ -962,7 +962,7 @@
         <v>16.43</v>
       </c>
       <c r="E35" t="n">
-        <v>202.030665732481</v>
+        <v>202.03</v>
       </c>
     </row>
     <row r="36">
@@ -979,7 +979,7 @@
         <v>15.48</v>
       </c>
       <c r="E36" t="n">
-        <v>73.3302152667139</v>
+        <v>73.33</v>
       </c>
     </row>
     <row r="37">
@@ -996,7 +996,7 @@
         <v>18.53</v>
       </c>
       <c r="E37" t="n">
-        <v>214.073195610809</v>
+        <v>214.07</v>
       </c>
     </row>
     <row r="38">
@@ -1013,7 +1013,7 @@
         <v>17.4</v>
       </c>
       <c r="E38" t="n">
-        <v>42.53223372865</v>
+        <v>42.53</v>
       </c>
     </row>
     <row r="39">
@@ -1030,7 +1030,7 @@
         <v>15.59</v>
       </c>
       <c r="E39" t="n">
-        <v>369.994982397467</v>
+        <v>369.99</v>
       </c>
     </row>
     <row r="40">
@@ -1047,7 +1047,7 @@
         <v>16.37</v>
       </c>
       <c r="E40" t="n">
-        <v>63.7652168345018</v>
+        <v>63.77</v>
       </c>
     </row>
     <row r="41">
@@ -1064,7 +1064,7 @@
         <v>15.05</v>
       </c>
       <c r="E41" t="n">
-        <v>389.151167553099</v>
+        <v>389.15</v>
       </c>
     </row>
     <row r="42">
@@ -1081,7 +1081,7 @@
         <v>18.1</v>
       </c>
       <c r="E42" t="n">
-        <v>1333.02720096251</v>
+        <v>1333.03</v>
       </c>
     </row>
     <row r="43">
@@ -1098,7 +1098,7 @@
         <v>14.53</v>
       </c>
       <c r="E43" t="n">
-        <v>158.727726863538</v>
+        <v>158.73</v>
       </c>
     </row>
     <row r="44">
@@ -1115,7 +1115,7 @@
         <v>14.79</v>
       </c>
       <c r="E44" t="n">
-        <v>207.648343905185</v>
+        <v>207.65</v>
       </c>
     </row>
     <row r="45">
@@ -1132,7 +1132,7 @@
         <v>16.74</v>
       </c>
       <c r="E45" t="n">
-        <v>79.9430192625256</v>
+        <v>79.94</v>
       </c>
     </row>
     <row r="46">
@@ -1149,7 +1149,7 @@
         <v>17.98</v>
       </c>
       <c r="E46" t="n">
-        <v>141.623474372649</v>
+        <v>141.62</v>
       </c>
     </row>
     <row r="47">
@@ -1166,7 +1166,7 @@
         <v>14.45</v>
       </c>
       <c r="E47" t="n">
-        <v>52.6564191605655</v>
+        <v>52.66</v>
       </c>
     </row>
     <row r="48">
@@ -1183,7 +1183,7 @@
         <v>15.47</v>
       </c>
       <c r="E48" t="n">
-        <v>286.334831463775</v>
+        <v>286.33</v>
       </c>
     </row>
     <row r="49">
@@ -1200,7 +1200,7 @@
         <v>13.27</v>
       </c>
       <c r="E49" t="n">
-        <v>1139.92549024171</v>
+        <v>1139.93</v>
       </c>
     </row>
     <row r="50">
@@ -1217,7 +1217,7 @@
         <v>12.97</v>
       </c>
       <c r="E50" t="n">
-        <v>558.831675284408</v>
+        <v>558.83</v>
       </c>
     </row>
     <row r="51">
@@ -1234,7 +1234,7 @@
         <v>12.86</v>
       </c>
       <c r="E51" t="n">
-        <v>398.82131708698</v>
+        <v>398.82</v>
       </c>
     </row>
     <row r="52">
@@ -1251,7 +1251,7 @@
         <v>19.14</v>
       </c>
       <c r="E52" t="n">
-        <v>68.3580436354788</v>
+        <v>68.36</v>
       </c>
     </row>
     <row r="53">
@@ -1268,7 +1268,7 @@
         <v>16.42</v>
       </c>
       <c r="E53" t="n">
-        <v>86.1025975090735</v>
+        <v>86.1</v>
       </c>
     </row>
     <row r="54">
@@ -1285,7 +1285,7 @@
         <v>14.55</v>
       </c>
       <c r="E54" t="n">
-        <v>1216.5281362054</v>
+        <v>1216.53</v>
       </c>
     </row>
     <row r="55">
@@ -1302,7 +1302,7 @@
         <v>20</v>
       </c>
       <c r="E55" t="n">
-        <v>131.594665698285</v>
+        <v>131.59</v>
       </c>
     </row>
     <row r="56">
@@ -1319,7 +1319,7 @@
         <v>16.03</v>
       </c>
       <c r="E56" t="n">
-        <v>41.0362503168788</v>
+        <v>41.04</v>
       </c>
     </row>
     <row r="57">
@@ -1336,7 +1336,7 @@
         <v>11.88</v>
       </c>
       <c r="E57" t="n">
-        <v>538.806128878053</v>
+        <v>538.81</v>
       </c>
     </row>
     <row r="58">
@@ -1353,7 +1353,7 @@
         <v>15.59</v>
       </c>
       <c r="E58" t="n">
-        <v>764.976546646818</v>
+        <v>764.98</v>
       </c>
     </row>
     <row r="59">
@@ -1370,7 +1370,7 @@
         <v>15.39</v>
       </c>
       <c r="E59" t="n">
-        <v>97.3456766430028</v>
+        <v>97.35</v>
       </c>
     </row>
     <row r="60">
@@ -1387,7 +1387,7 @@
         <v>13.12</v>
       </c>
       <c r="E60" t="n">
-        <v>160.614844743453</v>
+        <v>160.61</v>
       </c>
     </row>
     <row r="61">
@@ -1404,7 +1404,7 @@
         <v>14.67</v>
       </c>
       <c r="E61" t="n">
-        <v>106.737368936117</v>
+        <v>106.74</v>
       </c>
     </row>
     <row r="62">
@@ -1421,7 +1421,7 @@
         <v>17.36</v>
       </c>
       <c r="E62" t="n">
-        <v>509.599584107201</v>
+        <v>509.6</v>
       </c>
     </row>
     <row r="63">
@@ -1438,7 +1438,7 @@
         <v>14.72</v>
       </c>
       <c r="E63" t="n">
-        <v>63.7575300082552</v>
+        <v>63.76</v>
       </c>
     </row>
     <row r="64">
@@ -1455,7 +1455,7 @@
         <v>14</v>
       </c>
       <c r="E64" t="n">
-        <v>141.114198708223</v>
+        <v>141.11</v>
       </c>
     </row>
     <row r="65">
@@ -1472,7 +1472,7 @@
         <v>14.76</v>
       </c>
       <c r="E65" t="n">
-        <v>256.196022556866</v>
+        <v>256.2</v>
       </c>
     </row>
     <row r="66">
@@ -1489,7 +1489,7 @@
         <v>16.96</v>
       </c>
       <c r="E66" t="n">
-        <v>125.068531345796</v>
+        <v>125.07</v>
       </c>
     </row>
     <row r="67">
@@ -1506,7 +1506,7 @@
         <v>17.05</v>
       </c>
       <c r="E67" t="n">
-        <v>81.2848635291989</v>
+        <v>81.28</v>
       </c>
     </row>
     <row r="68">
@@ -1523,7 +1523,7 @@
         <v>16.91</v>
       </c>
       <c r="E68" t="n">
-        <v>83.5427432034627</v>
+        <v>83.54</v>
       </c>
     </row>
     <row r="69">
@@ -1540,7 +1540,7 @@
         <v>13.28</v>
       </c>
       <c r="E69" t="n">
-        <v>122.629127433793</v>
+        <v>122.63</v>
       </c>
     </row>
     <row r="70">
@@ -1557,7 +1557,7 @@
         <v>17.52</v>
       </c>
       <c r="E70" t="n">
-        <v>83.5877709062878</v>
+        <v>83.59</v>
       </c>
     </row>
     <row r="71">
@@ -1574,7 +1574,7 @@
         <v>13.39</v>
       </c>
       <c r="E71" t="n">
-        <v>904.312447076019</v>
+        <v>904.31</v>
       </c>
     </row>
     <row r="72">
@@ -1591,7 +1591,7 @@
         <v>17.59</v>
       </c>
       <c r="E72" t="n">
-        <v>236.435005251914</v>
+        <v>236.44</v>
       </c>
     </row>
     <row r="73">
@@ -1608,7 +1608,7 @@
         <v>17.77</v>
       </c>
       <c r="E73" t="n">
-        <v>118.991970097524</v>
+        <v>118.99</v>
       </c>
     </row>
     <row r="74">
@@ -1625,7 +1625,7 @@
         <v>16.5</v>
       </c>
       <c r="E74" t="n">
-        <v>65.7191011014196</v>
+        <v>65.72</v>
       </c>
     </row>
     <row r="75">
@@ -1642,7 +1642,7 @@
         <v>15.75</v>
       </c>
       <c r="E75" t="n">
-        <v>85.3182275372247</v>
+        <v>85.32</v>
       </c>
     </row>
     <row r="76">
@@ -1659,7 +1659,7 @@
         <v>16.12</v>
       </c>
       <c r="E76" t="n">
-        <v>133.146803068478</v>
+        <v>133.15</v>
       </c>
     </row>
     <row r="77">
@@ -1676,7 +1676,7 @@
         <v>15.34</v>
       </c>
       <c r="E77" t="n">
-        <v>69.7905275810356</v>
+        <v>69.79</v>
       </c>
     </row>
     <row r="78">
@@ -1693,7 +1693,7 @@
         <v>15.83</v>
       </c>
       <c r="E78" t="n">
-        <v>80.1993376016336</v>
+        <v>80.2</v>
       </c>
     </row>
     <row r="79">
@@ -1710,7 +1710,7 @@
         <v>14.37</v>
       </c>
       <c r="E79" t="n">
-        <v>22.1003260885369</v>
+        <v>22.1</v>
       </c>
     </row>
     <row r="80">
@@ -1727,7 +1727,7 @@
         <v>16.31</v>
       </c>
       <c r="E80" t="n">
-        <v>212.908460542169</v>
+        <v>212.91</v>
       </c>
     </row>
     <row r="81">
@@ -1744,7 +1744,7 @@
         <v>14.95</v>
       </c>
       <c r="E81" t="n">
-        <v>179.204637354441</v>
+        <v>179.2</v>
       </c>
     </row>
     <row r="82">
@@ -1761,7 +1761,7 @@
         <v>14.47</v>
       </c>
       <c r="E82" t="n">
-        <v>31.6382442319378</v>
+        <v>31.64</v>
       </c>
     </row>
     <row r="83">
@@ -1778,7 +1778,7 @@
         <v>12.94</v>
       </c>
       <c r="E83" t="n">
-        <v>327.958741949703</v>
+        <v>327.96</v>
       </c>
     </row>
     <row r="84">
@@ -1795,7 +1795,7 @@
         <v>13.66</v>
       </c>
       <c r="E84" t="n">
-        <v>114.416245790276</v>
+        <v>114.42</v>
       </c>
     </row>
     <row r="85">
@@ -1812,7 +1812,7 @@
         <v>11.82</v>
       </c>
       <c r="E85" t="n">
-        <v>56.8609935577368</v>
+        <v>56.86</v>
       </c>
     </row>
     <row r="86">
@@ -1829,7 +1829,7 @@
         <v>17.68</v>
       </c>
       <c r="E86" t="n">
-        <v>528.974480685149</v>
+        <v>528.97</v>
       </c>
     </row>
     <row r="87">
@@ -1846,7 +1846,7 @@
         <v>18.66</v>
       </c>
       <c r="E87" t="n">
-        <v>44.783634190953</v>
+        <v>44.78</v>
       </c>
     </row>
     <row r="88">
@@ -1863,7 +1863,7 @@
         <v>18.3</v>
       </c>
       <c r="E88" t="n">
-        <v>36.4515807449904</v>
+        <v>36.45</v>
       </c>
     </row>
     <row r="89">
@@ -1880,7 +1880,7 @@
         <v>18.79</v>
       </c>
       <c r="E89" t="n">
-        <v>106.701423888552</v>
+        <v>106.7</v>
       </c>
     </row>
     <row r="90">
@@ -1897,7 +1897,7 @@
         <v>15.17</v>
       </c>
       <c r="E90" t="n">
-        <v>956.735763083221</v>
+        <v>956.74</v>
       </c>
     </row>
     <row r="91">
@@ -1914,7 +1914,7 @@
         <v>19.04</v>
       </c>
       <c r="E91" t="n">
-        <v>57.0222918847161</v>
+        <v>57.02</v>
       </c>
     </row>
     <row r="92">
@@ -1931,7 +1931,7 @@
         <v>17.86</v>
       </c>
       <c r="E92" t="n">
-        <v>307.287850202986</v>
+        <v>307.29</v>
       </c>
     </row>
     <row r="93">
@@ -1948,7 +1948,7 @@
         <v>12.72</v>
       </c>
       <c r="E93" t="n">
-        <v>449.396925886893</v>
+        <v>449.4</v>
       </c>
     </row>
     <row r="94">
@@ -1965,7 +1965,7 @@
         <v>16.11</v>
       </c>
       <c r="E94" t="n">
-        <v>422.293746923865</v>
+        <v>422.29</v>
       </c>
     </row>
     <row r="95">
@@ -1982,7 +1982,7 @@
         <v>12.76</v>
       </c>
       <c r="E95" t="n">
-        <v>238.612421855381</v>
+        <v>238.61</v>
       </c>
     </row>
     <row r="96">
@@ -1999,7 +1999,7 @@
         <v>16.48</v>
       </c>
       <c r="E96" t="n">
-        <v>258.779227555316</v>
+        <v>258.78</v>
       </c>
     </row>
     <row r="97">
@@ -2016,7 +2016,7 @@
         <v>15.15</v>
       </c>
       <c r="E97" t="n">
-        <v>65.3565552409026</v>
+        <v>65.36</v>
       </c>
     </row>
     <row r="98">
@@ -2033,7 +2033,7 @@
         <v>14.77</v>
       </c>
       <c r="E98" t="n">
-        <v>260.091547243054</v>
+        <v>260.09</v>
       </c>
     </row>
     <row r="99">
@@ -2050,7 +2050,7 @@
         <v>17.27</v>
       </c>
       <c r="E99" t="n">
-        <v>105.627297931158</v>
+        <v>105.63</v>
       </c>
     </row>
     <row r="100">
@@ -2067,7 +2067,7 @@
         <v>13.98</v>
       </c>
       <c r="E100" t="n">
-        <v>49.8664994325906</v>
+        <v>49.87</v>
       </c>
     </row>
     <row r="101">
@@ -2084,7 +2084,7 @@
         <v>14.38</v>
       </c>
       <c r="E101" t="n">
-        <v>84.4659179040823</v>
+        <v>84.47</v>
       </c>
     </row>
     <row r="102">
@@ -2101,7 +2101,7 @@
         <v>19.76</v>
       </c>
       <c r="E102" t="n">
-        <v>51.7817235471195</v>
+        <v>51.78</v>
       </c>
     </row>
     <row r="103">
@@ -2118,7 +2118,7 @@
         <v>18.34</v>
       </c>
       <c r="E103" t="n">
-        <v>338.621489574043</v>
+        <v>338.62</v>
       </c>
     </row>
     <row r="104">
@@ -2135,7 +2135,7 @@
         <v>21.51</v>
       </c>
       <c r="E104" t="n">
-        <v>31.0879134773189</v>
+        <v>31.09</v>
       </c>
     </row>
     <row r="105">
@@ -2152,7 +2152,7 @@
         <v>18.88</v>
       </c>
       <c r="E105" t="n">
-        <v>1701.64874599703</v>
+        <v>1701.65</v>
       </c>
     </row>
     <row r="106">
@@ -2169,7 +2169,7 @@
         <v>19.88</v>
       </c>
       <c r="E106" t="n">
-        <v>66.0972426262876</v>
+        <v>66.1</v>
       </c>
     </row>
     <row r="107">
@@ -2186,7 +2186,7 @@
         <v>20.78</v>
       </c>
       <c r="E107" t="n">
-        <v>57.173434777996</v>
+        <v>57.17</v>
       </c>
     </row>
     <row r="108">
@@ -2203,7 +2203,7 @@
         <v>16.54</v>
       </c>
       <c r="E108" t="n">
-        <v>74.2084546085946</v>
+        <v>74.21</v>
       </c>
     </row>
     <row r="109">
@@ -2220,7 +2220,7 @@
         <v>16.3</v>
       </c>
       <c r="E109" t="n">
-        <v>144.010192772478</v>
+        <v>144.01</v>
       </c>
     </row>
     <row r="110">
@@ -2237,7 +2237,7 @@
         <v>23.53</v>
       </c>
       <c r="E110" t="n">
-        <v>42.4817305844879</v>
+        <v>42.48</v>
       </c>
     </row>
     <row r="111">
@@ -2254,7 +2254,7 @@
         <v>19.95</v>
       </c>
       <c r="E111" t="n">
-        <v>454.157418824854</v>
+        <v>454.16</v>
       </c>
     </row>
     <row r="112">
@@ -2271,7 +2271,7 @@
         <v>19.71</v>
       </c>
       <c r="E112" t="n">
-        <v>481.546939094501</v>
+        <v>481.55</v>
       </c>
     </row>
     <row r="113">
@@ -2288,7 +2288,7 @@
         <v>20.3</v>
       </c>
       <c r="E113" t="n">
-        <v>171.396264513103</v>
+        <v>171.4</v>
       </c>
     </row>
     <row r="114">
@@ -2305,7 +2305,7 @@
         <v>24.13</v>
       </c>
       <c r="E114" t="n">
-        <v>41.0769795979215</v>
+        <v>41.08</v>
       </c>
     </row>
     <row r="115">
@@ -2322,7 +2322,7 @@
         <v>18.08</v>
       </c>
       <c r="E115" t="n">
-        <v>167.712397173219</v>
+        <v>167.71</v>
       </c>
     </row>
     <row r="116">
@@ -2339,7 +2339,7 @@
         <v>23.49</v>
       </c>
       <c r="E116" t="n">
-        <v>287.130323562999</v>
+        <v>287.13</v>
       </c>
     </row>
     <row r="117">
@@ -2356,7 +2356,7 @@
         <v>19.42</v>
       </c>
       <c r="E117" t="n">
-        <v>489.385367046122</v>
+        <v>489.39</v>
       </c>
     </row>
     <row r="118">
@@ -2373,7 +2373,7 @@
         <v>20.09</v>
       </c>
       <c r="E118" t="n">
-        <v>28.9625977922901</v>
+        <v>28.96</v>
       </c>
     </row>
     <row r="119">
@@ -2390,7 +2390,7 @@
         <v>18.03</v>
       </c>
       <c r="E119" t="n">
-        <v>28.1674291057018</v>
+        <v>28.17</v>
       </c>
     </row>
     <row r="120">
@@ -2407,7 +2407,7 @@
         <v>16.29</v>
       </c>
       <c r="E120" t="n">
-        <v>255.842101170542</v>
+        <v>255.84</v>
       </c>
     </row>
     <row r="121">
@@ -2424,7 +2424,7 @@
         <v>20.28</v>
       </c>
       <c r="E121" t="n">
-        <v>163.010792902763</v>
+        <v>163.01</v>
       </c>
     </row>
     <row r="122">
@@ -2441,7 +2441,7 @@
         <v>20.34</v>
       </c>
       <c r="E122" t="n">
-        <v>757.26977393523</v>
+        <v>757.27</v>
       </c>
     </row>
     <row r="123">
@@ -2458,7 +2458,7 @@
         <v>20.4</v>
       </c>
       <c r="E123" t="n">
-        <v>406.633660969245</v>
+        <v>406.63</v>
       </c>
     </row>
     <row r="124">
@@ -2475,7 +2475,7 @@
         <v>22</v>
       </c>
       <c r="E124" t="n">
-        <v>35.0398788450239</v>
+        <v>35.04</v>
       </c>
     </row>
     <row r="125">
@@ -2492,7 +2492,7 @@
         <v>22.06</v>
       </c>
       <c r="E125" t="n">
-        <v>162.70013360406</v>
+        <v>162.7</v>
       </c>
     </row>
     <row r="126">
@@ -2509,7 +2509,7 @@
         <v>21.06</v>
       </c>
       <c r="E126" t="n">
-        <v>73.3825313157111</v>
+        <v>73.38</v>
       </c>
     </row>
     <row r="127">
@@ -2526,7 +2526,7 @@
         <v>20.9</v>
       </c>
       <c r="E127" t="n">
-        <v>318.146771591428</v>
+        <v>318.15</v>
       </c>
     </row>
     <row r="128">
@@ -2543,7 +2543,7 @@
         <v>24.37</v>
       </c>
       <c r="E128" t="n">
-        <v>241.085737752276</v>
+        <v>241.09</v>
       </c>
     </row>
     <row r="129">
@@ -2560,7 +2560,7 @@
         <v>18.99</v>
       </c>
       <c r="E129" t="n">
-        <v>125.68248837009</v>
+        <v>125.68</v>
       </c>
     </row>
     <row r="130">
@@ -2577,7 +2577,7 @@
         <v>20.17</v>
       </c>
       <c r="E130" t="n">
-        <v>57.6903319150131</v>
+        <v>57.69</v>
       </c>
     </row>
     <row r="131">
@@ -2594,7 +2594,7 @@
         <v>21.4</v>
       </c>
       <c r="E131" t="n">
-        <v>32.3221825146871</v>
+        <v>32.32</v>
       </c>
     </row>
     <row r="132">
@@ -2611,7 +2611,7 @@
         <v>18.54</v>
       </c>
       <c r="E132" t="n">
-        <v>521.895174970247</v>
+        <v>521.9</v>
       </c>
     </row>
     <row r="133">
@@ -2628,7 +2628,7 @@
         <v>18.94</v>
       </c>
       <c r="E133" t="n">
-        <v>99.0022810835693</v>
+        <v>99</v>
       </c>
     </row>
     <row r="134">
@@ -2645,7 +2645,7 @@
         <v>20.65</v>
       </c>
       <c r="E134" t="n">
-        <v>226.714670809526</v>
+        <v>226.71</v>
       </c>
     </row>
     <row r="135">
@@ -2662,7 +2662,7 @@
         <v>21.02</v>
       </c>
       <c r="E135" t="n">
-        <v>121.660673889057</v>
+        <v>121.66</v>
       </c>
     </row>
     <row r="136">
@@ -2679,7 +2679,7 @@
         <v>22.08</v>
       </c>
       <c r="E136" t="n">
-        <v>429.30290284259</v>
+        <v>429.3</v>
       </c>
     </row>
     <row r="137">
@@ -2696,7 +2696,7 @@
         <v>17.63</v>
       </c>
       <c r="E137" t="n">
-        <v>584.599265863535</v>
+        <v>584.6</v>
       </c>
     </row>
     <row r="138">
@@ -2713,7 +2713,7 @@
         <v>20.46</v>
       </c>
       <c r="E138" t="n">
-        <v>127.338482327627</v>
+        <v>127.34</v>
       </c>
     </row>
     <row r="139">
@@ -2730,7 +2730,7 @@
         <v>20.07</v>
       </c>
       <c r="E139" t="n">
-        <v>68.6420883205641</v>
+        <v>68.64</v>
       </c>
     </row>
     <row r="140">
@@ -2747,7 +2747,7 @@
         <v>23.94</v>
       </c>
       <c r="E140" t="n">
-        <v>17.2107783187926</v>
+        <v>17.21</v>
       </c>
     </row>
     <row r="141">
@@ -2764,7 +2764,7 @@
         <v>20.89</v>
       </c>
       <c r="E141" t="n">
-        <v>40.6273574055993</v>
+        <v>40.63</v>
       </c>
     </row>
     <row r="142">
@@ -2781,7 +2781,7 @@
         <v>20.07</v>
       </c>
       <c r="E142" t="n">
-        <v>138.105310120901</v>
+        <v>138.11</v>
       </c>
     </row>
     <row r="143">
@@ -2798,7 +2798,7 @@
         <v>23.68</v>
       </c>
       <c r="E143" t="n">
-        <v>335.348642045035</v>
+        <v>335.35</v>
       </c>
     </row>
     <row r="144">
@@ -2815,7 +2815,7 @@
         <v>21.69</v>
       </c>
       <c r="E144" t="n">
-        <v>158.291308925875</v>
+        <v>158.29</v>
       </c>
     </row>
     <row r="145">
@@ -2832,7 +2832,7 @@
         <v>18.02</v>
       </c>
       <c r="E145" t="n">
-        <v>609.652699340448</v>
+        <v>609.65</v>
       </c>
     </row>
     <row r="146">
@@ -2849,7 +2849,7 @@
         <v>21.31</v>
       </c>
       <c r="E146" t="n">
-        <v>115.648878807451</v>
+        <v>115.65</v>
       </c>
     </row>
     <row r="147">
@@ -2866,7 +2866,7 @@
         <v>22.29</v>
       </c>
       <c r="E147" t="n">
-        <v>74.5065083891898</v>
+        <v>74.51</v>
       </c>
     </row>
     <row r="148">
@@ -2883,7 +2883,7 @@
         <v>22.24</v>
       </c>
       <c r="E148" t="n">
-        <v>109.928344419139</v>
+        <v>109.93</v>
       </c>
     </row>
     <row r="149">
@@ -2900,7 +2900,7 @@
         <v>17.77</v>
       </c>
       <c r="E149" t="n">
-        <v>57.7826786414191</v>
+        <v>57.78</v>
       </c>
     </row>
     <row r="150">
@@ -2917,7 +2917,7 @@
         <v>19.24</v>
       </c>
       <c r="E150" t="n">
-        <v>154.941774496483</v>
+        <v>154.94</v>
       </c>
     </row>
     <row r="151">
@@ -2934,7 +2934,7 @@
         <v>20.75</v>
       </c>
       <c r="E151" t="n">
-        <v>105.866325014157</v>
+        <v>105.87</v>
       </c>
     </row>
     <row r="152">
@@ -2951,7 +2951,7 @@
         <v>20.31</v>
       </c>
       <c r="E152" t="n">
-        <v>1007.04098643989</v>
+        <v>1007.04</v>
       </c>
     </row>
     <row r="153">
@@ -2968,7 +2968,7 @@
         <v>18.73</v>
       </c>
       <c r="E153" t="n">
-        <v>72.4621616360575</v>
+        <v>72.46</v>
       </c>
     </row>
     <row r="154">
@@ -2985,7 +2985,7 @@
         <v>22.07</v>
       </c>
       <c r="E154" t="n">
-        <v>142.729424927295</v>
+        <v>142.73</v>
       </c>
     </row>
     <row r="155">
@@ -3002,7 +3002,7 @@
         <v>18.54</v>
       </c>
       <c r="E155" t="n">
-        <v>80.2458993782025</v>
+        <v>80.25</v>
       </c>
     </row>
     <row r="156">
@@ -3019,7 +3019,7 @@
         <v>17.2</v>
       </c>
       <c r="E156" t="n">
-        <v>85.3730234470876</v>
+        <v>85.37</v>
       </c>
     </row>
     <row r="157">
@@ -3036,7 +3036,7 @@
         <v>22.83</v>
       </c>
       <c r="E157" t="n">
-        <v>382.574573030782</v>
+        <v>382.57</v>
       </c>
     </row>
     <row r="158">
@@ -3053,7 +3053,7 @@
         <v>18.41</v>
       </c>
       <c r="E158" t="n">
-        <v>62.9933789810074</v>
+        <v>62.99</v>
       </c>
     </row>
     <row r="159">
@@ -3070,7 +3070,7 @@
         <v>18.65</v>
       </c>
       <c r="E159" t="n">
-        <v>11.4842921872248</v>
+        <v>11.48</v>
       </c>
     </row>
     <row r="160">
@@ -3087,7 +3087,7 @@
         <v>18.62</v>
       </c>
       <c r="E160" t="n">
-        <v>901.356510696764</v>
+        <v>901.36</v>
       </c>
     </row>
     <row r="161">
@@ -3104,7 +3104,7 @@
         <v>23.36</v>
       </c>
       <c r="E161" t="n">
-        <v>194.517563422253</v>
+        <v>194.52</v>
       </c>
     </row>
     <row r="162">
@@ -3121,7 +3121,7 @@
         <v>21.17</v>
       </c>
       <c r="E162" t="n">
-        <v>92.3442043104428</v>
+        <v>92.34</v>
       </c>
     </row>
     <row r="163">
@@ -3138,7 +3138,7 @@
         <v>21.5</v>
       </c>
       <c r="E163" t="n">
-        <v>1663.41831610779</v>
+        <v>1663.42</v>
       </c>
     </row>
     <row r="164">
@@ -3155,7 +3155,7 @@
         <v>24.39</v>
       </c>
       <c r="E164" t="n">
-        <v>181.07304060951</v>
+        <v>181.07</v>
       </c>
     </row>
     <row r="165">
@@ -3172,7 +3172,7 @@
         <v>21.44</v>
       </c>
       <c r="E165" t="n">
-        <v>217.882906249623</v>
+        <v>217.88</v>
       </c>
     </row>
     <row r="166">
@@ -3189,7 +3189,7 @@
         <v>15.85</v>
       </c>
       <c r="E166" t="n">
-        <v>520.431215200407</v>
+        <v>520.43</v>
       </c>
     </row>
     <row r="167">
@@ -3206,7 +3206,7 @@
         <v>22.28</v>
       </c>
       <c r="E167" t="n">
-        <v>177.179593877921</v>
+        <v>177.18</v>
       </c>
     </row>
     <row r="168">
@@ -3223,7 +3223,7 @@
         <v>23.12</v>
       </c>
       <c r="E168" t="n">
-        <v>65.4174581095297</v>
+        <v>65.42</v>
       </c>
     </row>
     <row r="169">
@@ -3240,7 +3240,7 @@
         <v>18.3</v>
       </c>
       <c r="E169" t="n">
-        <v>115.442783311371</v>
+        <v>115.44</v>
       </c>
     </row>
     <row r="170">
@@ -3257,7 +3257,7 @@
         <v>22.1</v>
       </c>
       <c r="E170" t="n">
-        <v>119.82358422166</v>
+        <v>119.82</v>
       </c>
     </row>
     <row r="171">
@@ -3274,7 +3274,7 @@
         <v>22.43</v>
       </c>
       <c r="E171" t="n">
-        <v>122.27449965663</v>
+        <v>122.27</v>
       </c>
     </row>
     <row r="172">
@@ -3291,7 +3291,7 @@
         <v>21.53</v>
       </c>
       <c r="E172" t="n">
-        <v>114.814929020709</v>
+        <v>114.81</v>
       </c>
     </row>
     <row r="173">
@@ -3308,7 +3308,7 @@
         <v>19</v>
       </c>
       <c r="E173" t="n">
-        <v>28.6329112439507</v>
+        <v>28.63</v>
       </c>
     </row>
     <row r="174">
@@ -3325,7 +3325,7 @@
         <v>20.28</v>
       </c>
       <c r="E174" t="n">
-        <v>143.566338527602</v>
+        <v>143.57</v>
       </c>
     </row>
     <row r="175">
@@ -3342,7 +3342,7 @@
         <v>21.85</v>
       </c>
       <c r="E175" t="n">
-        <v>282.032274012912</v>
+        <v>282.03</v>
       </c>
     </row>
     <row r="176">
@@ -3359,7 +3359,7 @@
         <v>22.06</v>
       </c>
       <c r="E176" t="n">
-        <v>101.545895849423</v>
+        <v>101.55</v>
       </c>
     </row>
     <row r="177">
@@ -3376,7 +3376,7 @@
         <v>17.73</v>
       </c>
       <c r="E177" t="n">
-        <v>188.899473413507</v>
+        <v>188.9</v>
       </c>
     </row>
     <row r="178">
@@ -3393,7 +3393,7 @@
         <v>18.78</v>
       </c>
       <c r="E178" t="n">
-        <v>254.105123012718</v>
+        <v>254.11</v>
       </c>
     </row>
     <row r="179">
@@ -3410,7 +3410,7 @@
         <v>20.53</v>
       </c>
       <c r="E179" t="n">
-        <v>22.3791387730458</v>
+        <v>22.38</v>
       </c>
     </row>
     <row r="180">
@@ -3427,7 +3427,7 @@
         <v>22.26</v>
       </c>
       <c r="E180" t="n">
-        <v>334.121800104916</v>
+        <v>334.12</v>
       </c>
     </row>
     <row r="181">
@@ -3444,7 +3444,7 @@
         <v>21.88</v>
       </c>
       <c r="E181" t="n">
-        <v>262.31945019871</v>
+        <v>262.32</v>
       </c>
     </row>
     <row r="182">
@@ -3461,7 +3461,7 @@
         <v>24.37</v>
       </c>
       <c r="E182" t="n">
-        <v>46.6136803607249</v>
+        <v>46.61</v>
       </c>
     </row>
     <row r="183">
@@ -3478,7 +3478,7 @@
         <v>22.86</v>
       </c>
       <c r="E183" t="n">
-        <v>270.269312196791</v>
+        <v>270.27</v>
       </c>
     </row>
     <row r="184">
@@ -3495,7 +3495,7 @@
         <v>20.65</v>
       </c>
       <c r="E184" t="n">
-        <v>394.009324355873</v>
+        <v>394.01</v>
       </c>
     </row>
     <row r="185">
@@ -3512,7 +3512,7 @@
         <v>18.29</v>
       </c>
       <c r="E185" t="n">
-        <v>73.5304361875883</v>
+        <v>73.53</v>
       </c>
     </row>
     <row r="186">
@@ -3529,7 +3529,7 @@
         <v>19.54</v>
       </c>
       <c r="E186" t="n">
-        <v>382.299509996713</v>
+        <v>382.3</v>
       </c>
     </row>
     <row r="187">
@@ -3546,7 +3546,7 @@
         <v>23.05</v>
       </c>
       <c r="E187" t="n">
-        <v>50.5259064248603</v>
+        <v>50.53</v>
       </c>
     </row>
     <row r="188">
@@ -3563,7 +3563,7 @@
         <v>22.55</v>
       </c>
       <c r="E188" t="n">
-        <v>105.191017961926</v>
+        <v>105.19</v>
       </c>
     </row>
     <row r="189">
@@ -3580,7 +3580,7 @@
         <v>21.91</v>
       </c>
       <c r="E189" t="n">
-        <v>77.0825263529158</v>
+        <v>77.08</v>
       </c>
     </row>
     <row r="190">
@@ -3597,7 +3597,7 @@
         <v>23.69</v>
       </c>
       <c r="E190" t="n">
-        <v>81.3598057662272</v>
+        <v>81.36</v>
       </c>
     </row>
     <row r="191">
@@ -3614,7 +3614,7 @@
         <v>20.12</v>
       </c>
       <c r="E191" t="n">
-        <v>515.133232459457</v>
+        <v>515.13</v>
       </c>
     </row>
     <row r="192">
@@ -3631,7 +3631,7 @@
         <v>23.2</v>
       </c>
       <c r="E192" t="n">
-        <v>208.369822171315</v>
+        <v>208.37</v>
       </c>
     </row>
     <row r="193">
@@ -3648,7 +3648,7 @@
         <v>20.28</v>
       </c>
       <c r="E193" t="n">
-        <v>95.8037114484387</v>
+        <v>95.8</v>
       </c>
     </row>
     <row r="194">
@@ -3665,7 +3665,7 @@
         <v>21.11</v>
       </c>
       <c r="E194" t="n">
-        <v>1040.45778697251</v>
+        <v>1040.46</v>
       </c>
     </row>
     <row r="195">
@@ -3682,7 +3682,7 @@
         <v>18.46</v>
       </c>
       <c r="E195" t="n">
-        <v>233.525056889072</v>
+        <v>233.53</v>
       </c>
     </row>
     <row r="196">
@@ -3699,7 +3699,7 @@
         <v>18.58</v>
       </c>
       <c r="E196" t="n">
-        <v>197.919079143795</v>
+        <v>197.92</v>
       </c>
     </row>
     <row r="197">
@@ -3716,7 +3716,7 @@
         <v>20.56</v>
       </c>
       <c r="E197" t="n">
-        <v>319.291383777647</v>
+        <v>319.29</v>
       </c>
     </row>
     <row r="198">
@@ -3733,7 +3733,7 @@
         <v>17.35</v>
       </c>
       <c r="E198" t="n">
-        <v>257.919969076912</v>
+        <v>257.92</v>
       </c>
     </row>
     <row r="199">
@@ -3750,7 +3750,7 @@
         <v>21.02</v>
       </c>
       <c r="E199" t="n">
-        <v>157.13705649981</v>
+        <v>157.14</v>
       </c>
     </row>
     <row r="200">
@@ -3767,7 +3767,7 @@
         <v>20.2</v>
       </c>
       <c r="E200" t="n">
-        <v>12.4563932996611</v>
+        <v>12.46</v>
       </c>
     </row>
     <row r="201">
@@ -3784,7 +3784,7 @@
         <v>18.27</v>
       </c>
       <c r="E201" t="n">
-        <v>220.614285147443</v>
+        <v>220.61</v>
       </c>
     </row>
     <row r="202">
@@ -3801,7 +3801,7 @@
         <v>18.29</v>
       </c>
       <c r="E202" t="n">
-        <v>393.962980563886</v>
+        <v>393.96</v>
       </c>
     </row>
     <row r="203">
@@ -3818,7 +3818,7 @@
         <v>20.83</v>
       </c>
       <c r="E203" t="n">
-        <v>203.422982340904</v>
+        <v>203.42</v>
       </c>
     </row>
     <row r="204">
@@ -3835,7 +3835,7 @@
         <v>20.08</v>
       </c>
       <c r="E204" t="n">
-        <v>107.075979202014</v>
+        <v>107.08</v>
       </c>
     </row>
     <row r="205">
@@ -3852,7 +3852,7 @@
         <v>16.59</v>
       </c>
       <c r="E205" t="n">
-        <v>246.996337251094</v>
+        <v>247</v>
       </c>
     </row>
     <row r="206">
@@ -3869,7 +3869,7 @@
         <v>20.72</v>
       </c>
       <c r="E206" t="n">
-        <v>144.260364000828</v>
+        <v>144.26</v>
       </c>
     </row>
     <row r="207">
@@ -3886,7 +3886,7 @@
         <v>15.99</v>
       </c>
       <c r="E207" t="n">
-        <v>107.216132761858</v>
+        <v>107.22</v>
       </c>
     </row>
     <row r="208">
@@ -3903,7 +3903,7 @@
         <v>18.78</v>
       </c>
       <c r="E208" t="n">
-        <v>272.994044129398</v>
+        <v>272.99</v>
       </c>
     </row>
     <row r="209">
@@ -3920,7 +3920,7 @@
         <v>17.04</v>
       </c>
       <c r="E209" t="n">
-        <v>484.835281212316</v>
+        <v>484.84</v>
       </c>
     </row>
     <row r="210">
@@ -3937,7 +3937,7 @@
         <v>18.86</v>
       </c>
       <c r="E210" t="n">
-        <v>75.1232007207329</v>
+        <v>75.12</v>
       </c>
     </row>
     <row r="211">
@@ -3954,7 +3954,7 @@
         <v>17.58</v>
       </c>
       <c r="E211" t="n">
-        <v>540.868308227741</v>
+        <v>540.87</v>
       </c>
     </row>
     <row r="212">
@@ -3971,7 +3971,7 @@
         <v>18.46</v>
       </c>
       <c r="E212" t="n">
-        <v>1385.25929486031</v>
+        <v>1385.26</v>
       </c>
     </row>
     <row r="213">
@@ -3988,7 +3988,7 @@
         <v>15.12</v>
       </c>
       <c r="E213" t="n">
-        <v>44.5239556733933</v>
+        <v>44.52</v>
       </c>
     </row>
     <row r="214">
@@ -4005,7 +4005,7 @@
         <v>20.09</v>
       </c>
       <c r="E214" t="n">
-        <v>91.9347332067601</v>
+        <v>91.93</v>
       </c>
     </row>
     <row r="215">
@@ -4022,7 +4022,7 @@
         <v>17.02</v>
       </c>
       <c r="E215" t="n">
-        <v>40.9687967463406</v>
+        <v>40.97</v>
       </c>
     </row>
     <row r="216">
@@ -4039,7 +4039,7 @@
         <v>14.02</v>
       </c>
       <c r="E216" t="n">
-        <v>44.0191539376998</v>
+        <v>44.02</v>
       </c>
     </row>
     <row r="217">
@@ -4056,7 +4056,7 @@
         <v>15.72</v>
       </c>
       <c r="E217" t="n">
-        <v>335.650780645258</v>
+        <v>335.65</v>
       </c>
     </row>
     <row r="218">
@@ -4073,7 +4073,7 @@
         <v>16.61</v>
       </c>
       <c r="E218" t="n">
-        <v>312.579741607409</v>
+        <v>312.58</v>
       </c>
     </row>
     <row r="219">
@@ -4090,7 +4090,7 @@
         <v>18.64</v>
       </c>
       <c r="E219" t="n">
-        <v>673.915071721165</v>
+        <v>673.92</v>
       </c>
     </row>
     <row r="220">
@@ -4107,7 +4107,7 @@
         <v>17.55</v>
       </c>
       <c r="E220" t="n">
-        <v>212.262103870768</v>
+        <v>212.26</v>
       </c>
     </row>
     <row r="221">
@@ -4124,7 +4124,7 @@
         <v>18.17</v>
       </c>
       <c r="E221" t="n">
-        <v>131.554502270989</v>
+        <v>131.55</v>
       </c>
     </row>
     <row r="222">
@@ -4141,7 +4141,7 @@
         <v>17.14</v>
       </c>
       <c r="E222" t="n">
-        <v>304.794690898231</v>
+        <v>304.79</v>
       </c>
     </row>
     <row r="223">
@@ -4158,7 +4158,7 @@
         <v>18.45</v>
       </c>
       <c r="E223" t="n">
-        <v>570.930023466285</v>
+        <v>570.93</v>
       </c>
     </row>
     <row r="224">
@@ -4175,7 +4175,7 @@
         <v>19.5</v>
       </c>
       <c r="E224" t="n">
-        <v>220.351292373007</v>
+        <v>220.35</v>
       </c>
     </row>
     <row r="225">
@@ -4192,7 +4192,7 @@
         <v>21.02</v>
       </c>
       <c r="E225" t="n">
-        <v>83.4554024475024</v>
+        <v>83.46</v>
       </c>
     </row>
     <row r="226">
@@ -4209,7 +4209,7 @@
         <v>21.76</v>
       </c>
       <c r="E226" t="n">
-        <v>33.9685806240675</v>
+        <v>33.97</v>
       </c>
     </row>
     <row r="227">
@@ -4226,7 +4226,7 @@
         <v>18.48</v>
       </c>
       <c r="E227" t="n">
-        <v>58.3973085991545</v>
+        <v>58.4</v>
       </c>
     </row>
     <row r="228">
@@ -4243,7 +4243,7 @@
         <v>13.92</v>
       </c>
       <c r="E228" t="n">
-        <v>110.734891039235</v>
+        <v>110.73</v>
       </c>
     </row>
     <row r="229">
@@ -4260,7 +4260,7 @@
         <v>19.91</v>
       </c>
       <c r="E229" t="n">
-        <v>637.492560104346</v>
+        <v>637.49</v>
       </c>
     </row>
     <row r="230">
@@ -4277,7 +4277,7 @@
         <v>18.2</v>
       </c>
       <c r="E230" t="n">
-        <v>361.887986218427</v>
+        <v>361.89</v>
       </c>
     </row>
     <row r="231">
@@ -4294,7 +4294,7 @@
         <v>18.42</v>
       </c>
       <c r="E231" t="n">
-        <v>196.528708707482</v>
+        <v>196.53</v>
       </c>
     </row>
     <row r="232">
@@ -4311,7 +4311,7 @@
         <v>20.04</v>
       </c>
       <c r="E232" t="n">
-        <v>70.5357657264197</v>
+        <v>70.54</v>
       </c>
     </row>
     <row r="233">
@@ -4328,7 +4328,7 @@
         <v>18.89</v>
       </c>
       <c r="E233" t="n">
-        <v>291.070487249218</v>
+        <v>291.07</v>
       </c>
     </row>
     <row r="234">
@@ -4345,7 +4345,7 @@
         <v>18.73</v>
       </c>
       <c r="E234" t="n">
-        <v>10.8946735651542</v>
+        <v>10.89</v>
       </c>
     </row>
     <row r="235">
@@ -4362,7 +4362,7 @@
         <v>17.16</v>
       </c>
       <c r="E235" t="n">
-        <v>141.88154551955</v>
+        <v>141.88</v>
       </c>
     </row>
     <row r="236">
@@ -4379,7 +4379,7 @@
         <v>18.43</v>
       </c>
       <c r="E236" t="n">
-        <v>838.705725199429</v>
+        <v>838.71</v>
       </c>
     </row>
     <row r="237">
@@ -4396,7 +4396,7 @@
         <v>20.75</v>
       </c>
       <c r="E237" t="n">
-        <v>199.772651703551</v>
+        <v>199.77</v>
       </c>
     </row>
     <row r="238">
@@ -4413,7 +4413,7 @@
         <v>19.88</v>
       </c>
       <c r="E238" t="n">
-        <v>238.950610892262</v>
+        <v>238.95</v>
       </c>
     </row>
     <row r="239">
@@ -4430,7 +4430,7 @@
         <v>17.19</v>
       </c>
       <c r="E239" t="n">
-        <v>163.238723671842</v>
+        <v>163.24</v>
       </c>
     </row>
     <row r="240">
@@ -4447,7 +4447,7 @@
         <v>16.71</v>
       </c>
       <c r="E240" t="n">
-        <v>80.6410439127384</v>
+        <v>80.64</v>
       </c>
     </row>
     <row r="241">
@@ -4464,7 +4464,7 @@
         <v>18.79</v>
       </c>
       <c r="E241" t="n">
-        <v>128.564797828522</v>
+        <v>128.56</v>
       </c>
     </row>
     <row r="242">
@@ -4481,7 +4481,7 @@
         <v>17.54</v>
       </c>
       <c r="E242" t="n">
-        <v>258.763417035334</v>
+        <v>258.76</v>
       </c>
     </row>
     <row r="243">
@@ -4498,7 +4498,7 @@
         <v>17.48</v>
       </c>
       <c r="E243" t="n">
-        <v>97.2401719683259</v>
+        <v>97.24</v>
       </c>
     </row>
     <row r="244">
@@ -4515,7 +4515,7 @@
         <v>19.42</v>
       </c>
       <c r="E244" t="n">
-        <v>45.5122475263045</v>
+        <v>45.51</v>
       </c>
     </row>
     <row r="245">
@@ -4532,7 +4532,7 @@
         <v>14.28</v>
       </c>
       <c r="E245" t="n">
-        <v>588.803072797721</v>
+        <v>588.8</v>
       </c>
     </row>
     <row r="246">
@@ -4549,7 +4549,7 @@
         <v>16.45</v>
       </c>
       <c r="E246" t="n">
-        <v>136.496111583199</v>
+        <v>136.5</v>
       </c>
     </row>
     <row r="247">
@@ -4566,7 +4566,7 @@
         <v>18.61</v>
       </c>
       <c r="E247" t="n">
-        <v>253.710197766394</v>
+        <v>253.71</v>
       </c>
     </row>
     <row r="248">
@@ -4583,7 +4583,7 @@
         <v>17.85</v>
       </c>
       <c r="E248" t="n">
-        <v>345.404091898682</v>
+        <v>345.4</v>
       </c>
     </row>
     <row r="249">
@@ -4600,7 +4600,7 @@
         <v>18.28</v>
       </c>
       <c r="E249" t="n">
-        <v>23.557494490513</v>
+        <v>23.56</v>
       </c>
     </row>
     <row r="250">
@@ -4617,7 +4617,7 @@
         <v>16.49</v>
       </c>
       <c r="E250" t="n">
-        <v>158.086417078228</v>
+        <v>158.09</v>
       </c>
     </row>
     <row r="251">
@@ -4634,7 +4634,7 @@
         <v>17.67</v>
       </c>
       <c r="E251" t="n">
-        <v>137.131623485771</v>
+        <v>137.13</v>
       </c>
     </row>
     <row r="252">
@@ -4651,7 +4651,7 @@
         <v>18.63</v>
       </c>
       <c r="E252" t="n">
-        <v>180.893533221791</v>
+        <v>180.89</v>
       </c>
     </row>
     <row r="253">
@@ -4668,7 +4668,7 @@
         <v>21.59</v>
       </c>
       <c r="E253" t="n">
-        <v>129.240288687188</v>
+        <v>129.24</v>
       </c>
     </row>
     <row r="254">
@@ -4685,7 +4685,7 @@
         <v>19.81</v>
       </c>
       <c r="E254" t="n">
-        <v>72.7694562331124</v>
+        <v>72.77</v>
       </c>
     </row>
     <row r="255">
@@ -4702,7 +4702,7 @@
         <v>16.69</v>
       </c>
       <c r="E255" t="n">
-        <v>141.057340669341</v>
+        <v>141.06</v>
       </c>
     </row>
     <row r="256">
@@ -4719,7 +4719,7 @@
         <v>17.9</v>
       </c>
       <c r="E256" t="n">
-        <v>60.2774959829646</v>
+        <v>60.28</v>
       </c>
     </row>
     <row r="257">
@@ -4736,7 +4736,7 @@
         <v>17.21</v>
       </c>
       <c r="E257" t="n">
-        <v>68.5223829202787</v>
+        <v>68.52</v>
       </c>
     </row>
     <row r="258">
@@ -4753,7 +4753,7 @@
         <v>15.08</v>
       </c>
       <c r="E258" t="n">
-        <v>216.682195034533</v>
+        <v>216.68</v>
       </c>
     </row>
     <row r="259">
@@ -4770,7 +4770,7 @@
         <v>15.4</v>
       </c>
       <c r="E259" t="n">
-        <v>443.507119981457</v>
+        <v>443.51</v>
       </c>
     </row>
     <row r="260">
@@ -4787,7 +4787,7 @@
         <v>20.09</v>
       </c>
       <c r="E260" t="n">
-        <v>223.096179827344</v>
+        <v>223.1</v>
       </c>
     </row>
     <row r="261">
@@ -4804,7 +4804,7 @@
         <v>19.36</v>
       </c>
       <c r="E261" t="n">
-        <v>353.115356580473</v>
+        <v>353.12</v>
       </c>
     </row>
     <row r="262">
@@ -4821,7 +4821,7 @@
         <v>17.92</v>
       </c>
       <c r="E262" t="n">
-        <v>1264.55700833534</v>
+        <v>1264.56</v>
       </c>
     </row>
     <row r="263">
@@ -4838,7 +4838,7 @@
         <v>17.62</v>
       </c>
       <c r="E263" t="n">
-        <v>145.510421254991</v>
+        <v>145.51</v>
       </c>
     </row>
     <row r="264">
@@ -4855,7 +4855,7 @@
         <v>20.24</v>
       </c>
       <c r="E264" t="n">
-        <v>165.636340766245</v>
+        <v>165.64</v>
       </c>
     </row>
     <row r="265">
@@ -4872,7 +4872,7 @@
         <v>16.42</v>
       </c>
       <c r="E265" t="n">
-        <v>431.132384855587</v>
+        <v>431.13</v>
       </c>
     </row>
     <row r="266">
@@ -4889,7 +4889,7 @@
         <v>20.53</v>
       </c>
       <c r="E266" t="n">
-        <v>336.189175469901</v>
+        <v>336.19</v>
       </c>
     </row>
     <row r="267">
@@ -4906,7 +4906,7 @@
         <v>14.87</v>
       </c>
       <c r="E267" t="n">
-        <v>243.886804445663</v>
+        <v>243.89</v>
       </c>
     </row>
     <row r="268">
@@ -4923,7 +4923,7 @@
         <v>21.44</v>
       </c>
       <c r="E268" t="n">
-        <v>238.982571658634</v>
+        <v>238.98</v>
       </c>
     </row>
     <row r="269">
@@ -4940,7 +4940,7 @@
         <v>20.14</v>
       </c>
       <c r="E269" t="n">
-        <v>354.551401562679</v>
+        <v>354.55</v>
       </c>
     </row>
     <row r="270">
@@ -4957,7 +4957,7 @@
         <v>14.33</v>
       </c>
       <c r="E270" t="n">
-        <v>411.189108230962</v>
+        <v>411.19</v>
       </c>
     </row>
     <row r="271">
@@ -4974,7 +4974,7 @@
         <v>15.91</v>
       </c>
       <c r="E271" t="n">
-        <v>93.9107354141073</v>
+        <v>93.91</v>
       </c>
     </row>
     <row r="272">
@@ -4991,7 +4991,7 @@
         <v>19.58</v>
       </c>
       <c r="E272" t="n">
-        <v>58.999287469234</v>
+        <v>59</v>
       </c>
     </row>
     <row r="273">
@@ -5008,7 +5008,7 @@
         <v>19.62</v>
       </c>
       <c r="E273" t="n">
-        <v>83.9600610186674</v>
+        <v>83.96</v>
       </c>
     </row>
     <row r="274">
@@ -5025,7 +5025,7 @@
         <v>18.11</v>
       </c>
       <c r="E274" t="n">
-        <v>237.850727008128</v>
+        <v>237.85</v>
       </c>
     </row>
     <row r="275">
@@ -5042,7 +5042,7 @@
         <v>20.39</v>
       </c>
       <c r="E275" t="n">
-        <v>107.242677582911</v>
+        <v>107.24</v>
       </c>
     </row>
     <row r="276">
@@ -5059,7 +5059,7 @@
         <v>19.47</v>
       </c>
       <c r="E276" t="n">
-        <v>21.6857737887085</v>
+        <v>21.69</v>
       </c>
     </row>
     <row r="277">
@@ -5076,7 +5076,7 @@
         <v>16</v>
       </c>
       <c r="E277" t="n">
-        <v>45.1510670403517</v>
+        <v>45.15</v>
       </c>
     </row>
     <row r="278">
@@ -5093,7 +5093,7 @@
         <v>17.92</v>
       </c>
       <c r="E278" t="n">
-        <v>78.15969358554</v>
+        <v>78.16</v>
       </c>
     </row>
     <row r="279">
@@ -5110,7 +5110,7 @@
         <v>17.57</v>
       </c>
       <c r="E279" t="n">
-        <v>1688.89254182877</v>
+        <v>1688.89</v>
       </c>
     </row>
     <row r="280">
@@ -5127,7 +5127,7 @@
         <v>15.52</v>
       </c>
       <c r="E280" t="n">
-        <v>79.4468903757499</v>
+        <v>79.45</v>
       </c>
     </row>
     <row r="281">
@@ -5144,7 +5144,7 @@
         <v>20.12</v>
       </c>
       <c r="E281" t="n">
-        <v>114.613807677148</v>
+        <v>114.61</v>
       </c>
     </row>
     <row r="282">
@@ -5161,7 +5161,7 @@
         <v>16.11</v>
       </c>
       <c r="E282" t="n">
-        <v>222.467064080266</v>
+        <v>222.47</v>
       </c>
     </row>
     <row r="283">
@@ -5178,7 +5178,7 @@
         <v>16.1</v>
       </c>
       <c r="E283" t="n">
-        <v>224.396624719056</v>
+        <v>224.4</v>
       </c>
     </row>
     <row r="284">
@@ -5195,7 +5195,7 @@
         <v>18.65</v>
       </c>
       <c r="E284" t="n">
-        <v>377.220299138353</v>
+        <v>377.22</v>
       </c>
     </row>
     <row r="285">
@@ -5212,7 +5212,7 @@
         <v>16.94</v>
       </c>
       <c r="E285" t="n">
-        <v>34.2177486046988</v>
+        <v>34.22</v>
       </c>
     </row>
     <row r="286">
@@ -5229,7 +5229,7 @@
         <v>15.79</v>
       </c>
       <c r="E286" t="n">
-        <v>464.146284779243</v>
+        <v>464.15</v>
       </c>
     </row>
     <row r="287">
@@ -5246,7 +5246,7 @@
         <v>17.55</v>
       </c>
       <c r="E287" t="n">
-        <v>236.957999027463</v>
+        <v>236.96</v>
       </c>
     </row>
     <row r="288">
@@ -5263,7 +5263,7 @@
         <v>17.47</v>
       </c>
       <c r="E288" t="n">
-        <v>290.171392411558</v>
+        <v>290.17</v>
       </c>
     </row>
     <row r="289">
@@ -5280,7 +5280,7 @@
         <v>14.18</v>
       </c>
       <c r="E289" t="n">
-        <v>59.755503776313</v>
+        <v>59.76</v>
       </c>
     </row>
     <row r="290">
@@ -5297,7 +5297,7 @@
         <v>15.66</v>
       </c>
       <c r="E290" t="n">
-        <v>85.5956123611464</v>
+        <v>85.6</v>
       </c>
     </row>
     <row r="291">
@@ -5314,7 +5314,7 @@
         <v>17.64</v>
       </c>
       <c r="E291" t="n">
-        <v>23.4956512382643</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="292">
@@ -5331,7 +5331,7 @@
         <v>15.53</v>
       </c>
       <c r="E292" t="n">
-        <v>1612.64228609497</v>
+        <v>1612.64</v>
       </c>
     </row>
     <row r="293">
@@ -5348,7 +5348,7 @@
         <v>16.06</v>
       </c>
       <c r="E293" t="n">
-        <v>112.167962234341</v>
+        <v>112.17</v>
       </c>
     </row>
     <row r="294">
@@ -5365,7 +5365,7 @@
         <v>16.67</v>
       </c>
       <c r="E294" t="n">
-        <v>220.999678119633</v>
+        <v>221</v>
       </c>
     </row>
     <row r="295">
@@ -5382,7 +5382,7 @@
         <v>19.14</v>
       </c>
       <c r="E295" t="n">
-        <v>57.7097430455918</v>
+        <v>57.71</v>
       </c>
     </row>
     <row r="296">
@@ -5399,7 +5399,7 @@
         <v>17.09</v>
       </c>
       <c r="E296" t="n">
-        <v>377.240675269844</v>
+        <v>377.24</v>
       </c>
     </row>
     <row r="297">
@@ -5416,7 +5416,7 @@
         <v>15.87</v>
       </c>
       <c r="E297" t="n">
-        <v>301.030638294713</v>
+        <v>301.03</v>
       </c>
     </row>
     <row r="298">
@@ -5433,7 +5433,7 @@
         <v>19.99</v>
       </c>
       <c r="E298" t="n">
-        <v>70.9393206644189</v>
+        <v>70.94</v>
       </c>
     </row>
     <row r="299">
@@ -5450,7 +5450,7 @@
         <v>17.71</v>
       </c>
       <c r="E299" t="n">
-        <v>447.837747768906</v>
+        <v>447.84</v>
       </c>
     </row>
     <row r="300">
@@ -5467,7 +5467,7 @@
         <v>18.06</v>
       </c>
       <c r="E300" t="n">
-        <v>62.6342206904625</v>
+        <v>62.63</v>
       </c>
     </row>
     <row r="301">
@@ -5484,7 +5484,7 @@
         <v>16.3</v>
       </c>
       <c r="E301" t="n">
-        <v>75.5591860262337</v>
+        <v>75.56</v>
       </c>
     </row>
     <row r="302">
@@ -5501,7 +5501,7 @@
         <v>21.54</v>
       </c>
       <c r="E302" t="n">
-        <v>71.6540075242875</v>
+        <v>71.65</v>
       </c>
     </row>
     <row r="303">
@@ -5518,7 +5518,7 @@
         <v>25.42</v>
       </c>
       <c r="E303" t="n">
-        <v>388.187340271473</v>
+        <v>388.19</v>
       </c>
     </row>
     <row r="304">
@@ -5535,7 +5535,7 @@
         <v>25.71</v>
       </c>
       <c r="E304" t="n">
-        <v>251.002094329063</v>
+        <v>251</v>
       </c>
     </row>
     <row r="305">
@@ -5552,7 +5552,7 @@
         <v>20.21</v>
       </c>
       <c r="E305" t="n">
-        <v>122.598635413952</v>
+        <v>122.6</v>
       </c>
     </row>
     <row r="306">
@@ -5569,7 +5569,7 @@
         <v>24.72</v>
       </c>
       <c r="E306" t="n">
-        <v>422.803075234547</v>
+        <v>422.8</v>
       </c>
     </row>
     <row r="307">
@@ -5586,7 +5586,7 @@
         <v>20.66</v>
       </c>
       <c r="E307" t="n">
-        <v>91.3244952550643</v>
+        <v>91.32</v>
       </c>
     </row>
     <row r="308">
@@ -5603,7 +5603,7 @@
         <v>23.37</v>
       </c>
       <c r="E308" t="n">
-        <v>200.10681280105</v>
+        <v>200.11</v>
       </c>
     </row>
     <row r="309">
@@ -5620,7 +5620,7 @@
         <v>21.79</v>
       </c>
       <c r="E309" t="n">
-        <v>288.894744516793</v>
+        <v>288.89</v>
       </c>
     </row>
     <row r="310">
@@ -5637,7 +5637,7 @@
         <v>22.92</v>
       </c>
       <c r="E310" t="n">
-        <v>1039.28089338029</v>
+        <v>1039.28</v>
       </c>
     </row>
     <row r="311">
@@ -5654,7 +5654,7 @@
         <v>22.04</v>
       </c>
       <c r="E311" t="n">
-        <v>709.204271032776</v>
+        <v>709.2</v>
       </c>
     </row>
     <row r="312">
@@ -5671,7 +5671,7 @@
         <v>24.65</v>
       </c>
       <c r="E312" t="n">
-        <v>15.7490472823884</v>
+        <v>15.75</v>
       </c>
     </row>
     <row r="313">
@@ -5688,7 +5688,7 @@
         <v>24.91</v>
       </c>
       <c r="E313" t="n">
-        <v>91.7773235747273</v>
+        <v>91.78</v>
       </c>
     </row>
     <row r="314">
@@ -5705,7 +5705,7 @@
         <v>25.3</v>
       </c>
       <c r="E314" t="n">
-        <v>1244.46654431337</v>
+        <v>1244.47</v>
       </c>
     </row>
     <row r="315">
@@ -5722,7 +5722,7 @@
         <v>21.95</v>
       </c>
       <c r="E315" t="n">
-        <v>1065.68246028783</v>
+        <v>1065.68</v>
       </c>
     </row>
     <row r="316">
@@ -5739,7 +5739,7 @@
         <v>25.38</v>
       </c>
       <c r="E316" t="n">
-        <v>23.5617036520191</v>
+        <v>23.56</v>
       </c>
     </row>
     <row r="317">
@@ -5756,7 +5756,7 @@
         <v>21.93</v>
       </c>
       <c r="E317" t="n">
-        <v>445.956747459107</v>
+        <v>445.96</v>
       </c>
     </row>
     <row r="318">
@@ -5773,7 +5773,7 @@
         <v>23.39</v>
       </c>
       <c r="E318" t="n">
-        <v>263.830613423984</v>
+        <v>263.83</v>
       </c>
     </row>
     <row r="319">
@@ -5790,7 +5790,7 @@
         <v>22.74</v>
       </c>
       <c r="E319" t="n">
-        <v>83.3399336764441</v>
+        <v>83.34</v>
       </c>
     </row>
     <row r="320">
@@ -5807,7 +5807,7 @@
         <v>23.41</v>
       </c>
       <c r="E320" t="n">
-        <v>653.561147697531</v>
+        <v>653.56</v>
       </c>
     </row>
     <row r="321">
@@ -5824,7 +5824,7 @@
         <v>19.92</v>
       </c>
       <c r="E321" t="n">
-        <v>69.6599053188291</v>
+        <v>69.66</v>
       </c>
     </row>
     <row r="322">
@@ -5841,7 +5841,7 @@
         <v>21.05</v>
       </c>
       <c r="E322" t="n">
-        <v>24.5384313787126</v>
+        <v>24.54</v>
       </c>
     </row>
     <row r="323">
@@ -5858,7 +5858,7 @@
         <v>21.92</v>
       </c>
       <c r="E323" t="n">
-        <v>245.480270738684</v>
+        <v>245.48</v>
       </c>
     </row>
     <row r="324">
@@ -5875,7 +5875,7 @@
         <v>23.55</v>
       </c>
       <c r="E324" t="n">
-        <v>464.299083669613</v>
+        <v>464.3</v>
       </c>
     </row>
     <row r="325">
@@ -5892,7 +5892,7 @@
         <v>22.72</v>
       </c>
       <c r="E325" t="n">
-        <v>61.7046780046362</v>
+        <v>61.7</v>
       </c>
     </row>
     <row r="326">
@@ -5909,7 +5909,7 @@
         <v>24.07</v>
       </c>
       <c r="E326" t="n">
-        <v>64.945740385987</v>
+        <v>64.95</v>
       </c>
     </row>
     <row r="327">
@@ -5926,7 +5926,7 @@
         <v>19.02</v>
       </c>
       <c r="E327" t="n">
-        <v>214.419931228245</v>
+        <v>214.42</v>
       </c>
     </row>
     <row r="328">
@@ -5943,7 +5943,7 @@
         <v>21.1</v>
       </c>
       <c r="E328" t="n">
-        <v>435.384462658666</v>
+        <v>435.38</v>
       </c>
     </row>
     <row r="329">
@@ -5960,7 +5960,7 @@
         <v>22.38</v>
       </c>
       <c r="E329" t="n">
-        <v>504.8838632258</v>
+        <v>504.88</v>
       </c>
     </row>
     <row r="330">
@@ -5977,7 +5977,7 @@
         <v>23.32</v>
       </c>
       <c r="E330" t="n">
-        <v>342.212262192733</v>
+        <v>342.21</v>
       </c>
     </row>
     <row r="331">
@@ -5994,7 +5994,7 @@
         <v>24.51</v>
       </c>
       <c r="E331" t="n">
-        <v>244.321996937826</v>
+        <v>244.32</v>
       </c>
     </row>
     <row r="332">
@@ -6011,7 +6011,7 @@
         <v>25.98</v>
       </c>
       <c r="E332" t="n">
-        <v>107.584295014558</v>
+        <v>107.58</v>
       </c>
     </row>
     <row r="333">
@@ -6028,7 +6028,7 @@
         <v>21.04</v>
       </c>
       <c r="E333" t="n">
-        <v>107.739076326046</v>
+        <v>107.74</v>
       </c>
     </row>
     <row r="334">
@@ -6045,7 +6045,7 @@
         <v>21.85</v>
       </c>
       <c r="E334" t="n">
-        <v>188.367943270723</v>
+        <v>188.37</v>
       </c>
     </row>
     <row r="335">
@@ -6062,7 +6062,7 @@
         <v>20.15</v>
       </c>
       <c r="E335" t="n">
-        <v>251.308399087833</v>
+        <v>251.31</v>
       </c>
     </row>
     <row r="336">
@@ -6079,7 +6079,7 @@
         <v>23.07</v>
       </c>
       <c r="E336" t="n">
-        <v>235.609603445099</v>
+        <v>235.61</v>
       </c>
     </row>
     <row r="337">
@@ -6096,7 +6096,7 @@
         <v>22.43</v>
       </c>
       <c r="E337" t="n">
-        <v>63.1498234359013</v>
+        <v>63.15</v>
       </c>
     </row>
     <row r="338">
@@ -6113,7 +6113,7 @@
         <v>24.77</v>
       </c>
       <c r="E338" t="n">
-        <v>118.752651864807</v>
+        <v>118.75</v>
       </c>
     </row>
     <row r="339">
@@ -6130,7 +6130,7 @@
         <v>24.74</v>
       </c>
       <c r="E339" t="n">
-        <v>80.51615856989</v>
+        <v>80.52</v>
       </c>
     </row>
     <row r="340">
@@ -6147,7 +6147,7 @@
         <v>25.01</v>
       </c>
       <c r="E340" t="n">
-        <v>104.77499771068</v>
+        <v>104.77</v>
       </c>
     </row>
     <row r="341">
@@ -6164,7 +6164,7 @@
         <v>21.1</v>
       </c>
       <c r="E341" t="n">
-        <v>31.3919692248154</v>
+        <v>31.39</v>
       </c>
     </row>
     <row r="342">
@@ -6181,7 +6181,7 @@
         <v>21.72</v>
       </c>
       <c r="E342" t="n">
-        <v>76.3088940750719</v>
+        <v>76.31</v>
       </c>
     </row>
     <row r="343">
@@ -6198,7 +6198,7 @@
         <v>21.46</v>
       </c>
       <c r="E343" t="n">
-        <v>23.0266492938873</v>
+        <v>23.03</v>
       </c>
     </row>
     <row r="344">
@@ -6215,7 +6215,7 @@
         <v>23.92</v>
       </c>
       <c r="E344" t="n">
-        <v>136.441587763904</v>
+        <v>136.44</v>
       </c>
     </row>
     <row r="345">
@@ -6232,7 +6232,7 @@
         <v>22.45</v>
       </c>
       <c r="E345" t="n">
-        <v>210.453573465418</v>
+        <v>210.45</v>
       </c>
     </row>
     <row r="346">
@@ -6249,7 +6249,7 @@
         <v>27.92</v>
       </c>
       <c r="E346" t="n">
-        <v>472.850898608418</v>
+        <v>472.85</v>
       </c>
     </row>
     <row r="347">
@@ -6266,7 +6266,7 @@
         <v>23.18</v>
       </c>
       <c r="E347" t="n">
-        <v>49.7382191914699</v>
+        <v>49.74</v>
       </c>
     </row>
     <row r="348">
@@ -6283,7 +6283,7 @@
         <v>23.96</v>
       </c>
       <c r="E348" t="n">
-        <v>72.5864603979359</v>
+        <v>72.59</v>
       </c>
     </row>
     <row r="349">
@@ -6300,7 +6300,7 @@
         <v>22.14</v>
       </c>
       <c r="E349" t="n">
-        <v>123.363548777496</v>
+        <v>123.36</v>
       </c>
     </row>
     <row r="350">
@@ -6317,7 +6317,7 @@
         <v>23.94</v>
       </c>
       <c r="E350" t="n">
-        <v>99.5503749012441</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="351">
@@ -6334,7 +6334,7 @@
         <v>25</v>
       </c>
       <c r="E351" t="n">
-        <v>166.772510987973</v>
+        <v>166.77</v>
       </c>
     </row>
     <row r="352">
@@ -6351,7 +6351,7 @@
         <v>24.45</v>
       </c>
       <c r="E352" t="n">
-        <v>155.006040664971</v>
+        <v>155.01</v>
       </c>
     </row>
     <row r="353">
@@ -6368,7 +6368,7 @@
         <v>20.99</v>
       </c>
       <c r="E353" t="n">
-        <v>327.153052723624</v>
+        <v>327.15</v>
       </c>
     </row>
     <row r="354">
@@ -6385,7 +6385,7 @@
         <v>25.41</v>
       </c>
       <c r="E354" t="n">
-        <v>81.907288251821</v>
+        <v>81.91</v>
       </c>
     </row>
     <row r="355">
@@ -6402,7 +6402,7 @@
         <v>26.68</v>
       </c>
       <c r="E355" t="n">
-        <v>19.1308595536032</v>
+        <v>19.13</v>
       </c>
     </row>
     <row r="356">
@@ -6419,7 +6419,7 @@
         <v>24.68</v>
       </c>
       <c r="E356" t="n">
-        <v>39.3686325589894</v>
+        <v>39.37</v>
       </c>
     </row>
     <row r="357">
@@ -6436,7 +6436,7 @@
         <v>23.46</v>
       </c>
       <c r="E357" t="n">
-        <v>143.149874767478</v>
+        <v>143.15</v>
       </c>
     </row>
     <row r="358">
@@ -6453,7 +6453,7 @@
         <v>22.57</v>
       </c>
       <c r="E358" t="n">
-        <v>329.136511931103</v>
+        <v>329.14</v>
       </c>
     </row>
     <row r="359">
@@ -6470,7 +6470,7 @@
         <v>21.87</v>
       </c>
       <c r="E359" t="n">
-        <v>319.105805624835</v>
+        <v>319.11</v>
       </c>
     </row>
     <row r="360">
@@ -6487,7 +6487,7 @@
         <v>22.92</v>
       </c>
       <c r="E360" t="n">
-        <v>63.8115287500501</v>
+        <v>63.81</v>
       </c>
     </row>
     <row r="361">
@@ -6504,7 +6504,7 @@
         <v>21.43</v>
       </c>
       <c r="E361" t="n">
-        <v>65.8094880596617</v>
+        <v>65.81</v>
       </c>
     </row>
     <row r="362">
@@ -6521,7 +6521,7 @@
         <v>21.94</v>
       </c>
       <c r="E362" t="n">
-        <v>46.7557801613566</v>
+        <v>46.76</v>
       </c>
     </row>
     <row r="363">
@@ -6538,7 +6538,7 @@
         <v>25.25</v>
       </c>
       <c r="E363" t="n">
-        <v>261.757879766146</v>
+        <v>261.76</v>
       </c>
     </row>
     <row r="364">
@@ -6555,7 +6555,7 @@
         <v>23.07</v>
       </c>
       <c r="E364" t="n">
-        <v>649.356146824113</v>
+        <v>649.36</v>
       </c>
     </row>
     <row r="365">
@@ -6572,7 +6572,7 @@
         <v>21.38</v>
       </c>
       <c r="E365" t="n">
-        <v>265.712430618291</v>
+        <v>265.71</v>
       </c>
     </row>
     <row r="366">
@@ -6589,7 +6589,7 @@
         <v>20.67</v>
       </c>
       <c r="E366" t="n">
-        <v>48.6974725881171</v>
+        <v>48.7</v>
       </c>
     </row>
     <row r="367">
@@ -6606,7 +6606,7 @@
         <v>22.09</v>
       </c>
       <c r="E367" t="n">
-        <v>227.287048999137</v>
+        <v>227.29</v>
       </c>
     </row>
     <row r="368">
@@ -6623,7 +6623,7 @@
         <v>22.31</v>
       </c>
       <c r="E368" t="n">
-        <v>320.634052704095</v>
+        <v>320.63</v>
       </c>
     </row>
     <row r="369">
@@ -6640,7 +6640,7 @@
         <v>25.23</v>
       </c>
       <c r="E369" t="n">
-        <v>123.529426265248</v>
+        <v>123.53</v>
       </c>
     </row>
     <row r="370">
@@ -6657,7 +6657,7 @@
         <v>23.23</v>
       </c>
       <c r="E370" t="n">
-        <v>138.815369009504</v>
+        <v>138.82</v>
       </c>
     </row>
     <row r="371">
@@ -6674,7 +6674,7 @@
         <v>23.55</v>
       </c>
       <c r="E371" t="n">
-        <v>178.185877573565</v>
+        <v>178.19</v>
       </c>
     </row>
     <row r="372">
@@ -6691,7 +6691,7 @@
         <v>19.94</v>
       </c>
       <c r="E372" t="n">
-        <v>350.59093481343</v>
+        <v>350.59</v>
       </c>
     </row>
     <row r="373">
@@ -6708,7 +6708,7 @@
         <v>23.29</v>
       </c>
       <c r="E373" t="n">
-        <v>44.0553334868564</v>
+        <v>44.06</v>
       </c>
     </row>
     <row r="374">
@@ -6725,7 +6725,7 @@
         <v>25.11</v>
       </c>
       <c r="E374" t="n">
-        <v>485.157687872565</v>
+        <v>485.16</v>
       </c>
     </row>
     <row r="375">
@@ -6742,7 +6742,7 @@
         <v>21.95</v>
       </c>
       <c r="E375" t="n">
-        <v>80.7532459176471</v>
+        <v>80.75</v>
       </c>
     </row>
     <row r="376">
@@ -6759,7 +6759,7 @@
         <v>22.93</v>
       </c>
       <c r="E376" t="n">
-        <v>380.824588164036</v>
+        <v>380.82</v>
       </c>
     </row>
     <row r="377">
@@ -6776,7 +6776,7 @@
         <v>23.27</v>
       </c>
       <c r="E377" t="n">
-        <v>215.391538886303</v>
+        <v>215.39</v>
       </c>
     </row>
     <row r="378">
@@ -6793,7 +6793,7 @@
         <v>20.38</v>
       </c>
       <c r="E378" t="n">
-        <v>334.490195925823</v>
+        <v>334.49</v>
       </c>
     </row>
     <row r="379">
@@ -6810,7 +6810,7 @@
         <v>24.09</v>
       </c>
       <c r="E379" t="n">
-        <v>619.003746988126</v>
+        <v>619</v>
       </c>
     </row>
     <row r="380">
@@ -6827,7 +6827,7 @@
         <v>21.45</v>
       </c>
       <c r="E380" t="n">
-        <v>894.190755097031</v>
+        <v>894.19</v>
       </c>
     </row>
     <row r="381">
@@ -6844,7 +6844,7 @@
         <v>23.2</v>
       </c>
       <c r="E381" t="n">
-        <v>21.0713945116081</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="382">
@@ -6861,7 +6861,7 @@
         <v>24.18</v>
       </c>
       <c r="E382" t="n">
-        <v>84.9523921402267</v>
+        <v>84.95</v>
       </c>
     </row>
     <row r="383">
@@ -6878,7 +6878,7 @@
         <v>24.58</v>
       </c>
       <c r="E383" t="n">
-        <v>43.1112046661957</v>
+        <v>43.11</v>
       </c>
     </row>
     <row r="384">
@@ -6895,7 +6895,7 @@
         <v>24.14</v>
       </c>
       <c r="E384" t="n">
-        <v>191.36468902992</v>
+        <v>191.36</v>
       </c>
     </row>
     <row r="385">
@@ -6912,7 +6912,7 @@
         <v>22.4</v>
       </c>
       <c r="E385" t="n">
-        <v>394.213445175744</v>
+        <v>394.21</v>
       </c>
     </row>
     <row r="386">
@@ -6929,7 +6929,7 @@
         <v>24.89</v>
       </c>
       <c r="E386" t="n">
-        <v>647.514168088255</v>
+        <v>647.51</v>
       </c>
     </row>
     <row r="387">
@@ -6946,7 +6946,7 @@
         <v>21.66</v>
       </c>
       <c r="E387" t="n">
-        <v>100.487894975881</v>
+        <v>100.49</v>
       </c>
     </row>
     <row r="388">
@@ -6963,7 +6963,7 @@
         <v>23.2</v>
       </c>
       <c r="E388" t="n">
-        <v>141.782024294885</v>
+        <v>141.78</v>
       </c>
     </row>
     <row r="389">
@@ -6980,7 +6980,7 @@
         <v>22.89</v>
       </c>
       <c r="E389" t="n">
-        <v>44.1661435241631</v>
+        <v>44.17</v>
       </c>
     </row>
     <row r="390">
@@ -6997,7 +6997,7 @@
         <v>22.73</v>
       </c>
       <c r="E390" t="n">
-        <v>339.194991250897</v>
+        <v>339.19</v>
       </c>
     </row>
     <row r="391">
@@ -7014,7 +7014,7 @@
         <v>21.15</v>
       </c>
       <c r="E391" t="n">
-        <v>33.4742192897725</v>
+        <v>33.47</v>
       </c>
     </row>
     <row r="392">
@@ -7031,7 +7031,7 @@
         <v>21.76</v>
       </c>
       <c r="E392" t="n">
-        <v>72.4245899053795</v>
+        <v>72.42</v>
       </c>
     </row>
     <row r="393">
@@ -7048,7 +7048,7 @@
         <v>24.9</v>
       </c>
       <c r="E393" t="n">
-        <v>590.758778806838</v>
+        <v>590.76</v>
       </c>
     </row>
     <row r="394">
@@ -7065,7 +7065,7 @@
         <v>21.37</v>
       </c>
       <c r="E394" t="n">
-        <v>357.971680608154</v>
+        <v>357.97</v>
       </c>
     </row>
     <row r="395">
@@ -7082,7 +7082,7 @@
         <v>22.67</v>
       </c>
       <c r="E395" t="n">
-        <v>31.2139721456778</v>
+        <v>31.21</v>
       </c>
     </row>
     <row r="396">
@@ -7099,7 +7099,7 @@
         <v>23.92</v>
       </c>
       <c r="E396" t="n">
-        <v>470.26290386353</v>
+        <v>470.26</v>
       </c>
     </row>
     <row r="397">
@@ -7116,7 +7116,7 @@
         <v>20.45</v>
       </c>
       <c r="E397" t="n">
-        <v>70.9623490246244</v>
+        <v>70.96</v>
       </c>
     </row>
     <row r="398">
@@ -7133,7 +7133,7 @@
         <v>21.03</v>
       </c>
       <c r="E398" t="n">
-        <v>91.5422028120055</v>
+        <v>91.54</v>
       </c>
     </row>
     <row r="399">
@@ -7150,7 +7150,7 @@
         <v>20.7</v>
       </c>
       <c r="E399" t="n">
-        <v>83.583403323177</v>
+        <v>83.58</v>
       </c>
     </row>
     <row r="400">
@@ -7167,7 +7167,7 @@
         <v>19.31</v>
       </c>
       <c r="E400" t="n">
-        <v>84.0240877720691</v>
+        <v>84.02</v>
       </c>
     </row>
     <row r="401">
@@ -7184,7 +7184,7 @@
         <v>27.1</v>
       </c>
       <c r="E401" t="n">
-        <v>27.5068842626427</v>
+        <v>27.51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>